<commit_message>
Data update for AOCoLUPpUA
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\land\AOCoLUPpUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD49024-32D5-45EB-8C27-7FDD535E413B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872242AB-5149-4801-8040-926211EDC1E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="811" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="811" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -931,7 +931,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1029,8 +1029,8 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="B11" s="12">
-        <f>B10/A18</f>
-        <v>277.23581768722721</v>
+        <f>B10*A18</f>
+        <v>457.63622493973321</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>40</v>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B2" s="3">
         <f>'Forest Mgmt Costs'!B11</f>
-        <v>277.23581768722721</v>
+        <v>457.63622493973321</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="B3" s="3">
         <f>'Forest Mgmt Costs'!B11</f>
-        <v>277.23581768722721</v>
+        <v>457.63622493973321</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Revert "Uploading newest EPS-US files"
This reverts commit 77b035798ee93ce6408f3bd1d4511e3b502cb2b2.
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,45 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\AOCoLUPpUA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94B7C1-28EB-4AAB-A6C5-9A13131631C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="AOCoLUPpUA" sheetId="3" r:id="rId2"/>
+    <sheet name="Forest Mgmt Costs" sheetId="4" r:id="rId2"/>
+    <sheet name="AOCoLUPpUA" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>AOCoLUPpUA Annual Ongoing Cost of Land Use Policies per Unit Area</t>
   </si>
@@ -50,6 +33,24 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>This variable is for the costs to maintain lands previously affected by one of the</t>
+  </si>
+  <si>
+    <t>avoid emission of sequestered CO2.</t>
+  </si>
+  <si>
+    <t>This variable is NOT for use with the Improved Forest Management policy,</t>
+  </si>
+  <si>
+    <t>as that policy must be repeated every year in order to obtain carbon benefits</t>
+  </si>
+  <si>
+    <t>in that year.  Its cost is handled in the "Implementation Cost of Land Use</t>
+  </si>
+  <si>
+    <t>Policies per Unit Area" variable.</t>
+  </si>
+  <si>
     <t>forest set asides</t>
   </si>
   <si>
@@ -71,26 +72,143 @@
     <t>annual maintenance cost ($ / acre)</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Based on consultation with the organization American Forests, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">annual ongoing for land affected by these policy levers is a </t>
-  </si>
-  <si>
-    <t>small part of lifetime costs. For this reason, we do not attempt</t>
-  </si>
-  <si>
-    <t>to track these in the US model.</t>
+    <t>Avoid deforestion, peatland restoration, and forest restoration policies</t>
+  </si>
+  <si>
+    <t>are not used in the U.S. version of the model.</t>
+  </si>
+  <si>
+    <t>land use policies (such as "Afforestation/Reforestation") and thereby</t>
+  </si>
+  <si>
+    <t>Table 2: Forest by Region (thousand acres)</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Softwood</t>
+  </si>
+  <si>
+    <t>Hardwood</t>
+  </si>
+  <si>
+    <t>Corn Belt</t>
+  </si>
+  <si>
+    <t>Lake States</t>
+  </si>
+  <si>
+    <t>Northeast</t>
+  </si>
+  <si>
+    <t>PNE</t>
+  </si>
+  <si>
+    <t>PNW</t>
+  </si>
+  <si>
+    <t>PSW</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Table 5: Cost per acre of forest management practices by region</t>
+  </si>
+  <si>
+    <t>Region and Practice</t>
+  </si>
+  <si>
+    <t>Stand Type</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Softwoods</t>
+  </si>
+  <si>
+    <t>Hardwoods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Decadal Management*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Precommercial thin</t>
+  </si>
+  <si>
+    <t>hardwoods value assumed to be zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fertilizer</t>
+  </si>
+  <si>
+    <t>hardwoods value calculated based on other area fertizlier costs and scaled relative to softwoods compared to other regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Herbicide</t>
+  </si>
+  <si>
+    <t>Cornbelt</t>
+  </si>
+  <si>
+    <t>values calculated based on other data in this table</t>
+  </si>
+  <si>
+    <t>*Decadal costs are annualized here</t>
+  </si>
+  <si>
+    <t>Calculated Average Forest Management Cost</t>
+  </si>
+  <si>
+    <t>2002$ / acre</t>
+  </si>
+  <si>
+    <t>U.S. Forest Service</t>
+  </si>
+  <si>
+    <t>Regional Cost Information for Private Timberland Conversion and Management</t>
+  </si>
+  <si>
+    <t>http://www.fs.fed.us/pnw/pubs/pnw-gtr684.pdf</t>
+  </si>
+  <si>
+    <t>Table 2 (forest area by region), Table 5 (management costs per acre by region)</t>
+  </si>
+  <si>
+    <t>Currency Year</t>
+  </si>
+  <si>
+    <t>We adjust the sources' dollars to 2012 dollars using the following conversion factors:</t>
+  </si>
+  <si>
+    <t>2002 to 2012, for U.S. Forest Service (2006) "Regional Cost Information…"</t>
+  </si>
+  <si>
+    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+  </si>
+  <si>
+    <t>2012$ / acre</t>
+  </si>
+  <si>
+    <t>Both new forests (from afforestation/reforestation) and forests set aside from</t>
+  </si>
+  <si>
+    <t>timber harvesting need to be managed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +218,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,13 +255,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -183,49 +323,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+  <cellStyles count="8">
+    <cellStyle name="Body: normal cell" xfId="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
+    <cellStyle name="Footnotes: top row" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="5"/>
+    <cellStyle name="Table title" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -331,7 +485,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,26 +518,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,23 +553,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -608,12 +728,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -627,61 +745,576 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.278</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>50+1614</f>
+        <v>1664</v>
+      </c>
+      <c r="C3">
+        <f>377+25502</f>
+        <v>25879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <f>972+4013</f>
+        <v>4985</v>
+      </c>
+      <c r="C4">
+        <f>2396+22953</f>
+        <v>25349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <f>3955+13315</f>
+        <v>17270</v>
+      </c>
+      <c r="C5">
+        <f>7041+45009</f>
+        <v>52050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <f>2879+2953</f>
+        <v>5832</v>
+      </c>
+      <c r="C6">
+        <f>119</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <f>6236+2826</f>
+        <v>9062</v>
+      </c>
+      <c r="C7">
+        <f>923+1277</f>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <f>2156+2707</f>
+        <v>4863</v>
+      </c>
+      <c r="C8">
+        <f>826+1748</f>
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <f>2918+12457</f>
+        <v>15375</v>
+      </c>
+      <c r="C9">
+        <f>8+2680</f>
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <f>15095+29814</f>
+        <v>44909</v>
+      </c>
+      <c r="C10">
+        <f>7434+52435</f>
+        <v>59869</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <f>10315+29977</f>
+        <v>40292</v>
+      </c>
+      <c r="C11">
+        <f>4193+30945</f>
+        <v>35138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <f>39/10</f>
+        <v>3.9</v>
+      </c>
+      <c r="C16">
+        <f>35.46/10</f>
+        <v>3.5460000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>95.55</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>44.67</v>
+      </c>
+      <c r="C18" s="10">
+        <f>C23*(B18/B23)</f>
+        <v>13.041950354609931</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>58.48</v>
+      </c>
+      <c r="C19">
+        <v>58.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <f>21.5/10</f>
+        <v>2.15</v>
+      </c>
+      <c r="C21">
+        <f>16.71/10</f>
+        <v>1.671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>65.11</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>50.76</v>
+      </c>
+      <c r="C23">
+        <v>14.82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>58.48</v>
+      </c>
+      <c r="C24">
+        <v>58.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <f>21.61/10</f>
+        <v>2.161</v>
+      </c>
+      <c r="C26">
+        <f>16.8/10</f>
+        <v>1.6800000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>65.11</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>50.76</v>
+      </c>
+      <c r="C28">
+        <v>14.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29">
+        <v>58.48</v>
+      </c>
+      <c r="C29">
+        <v>58.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <f>24.49/10</f>
+        <v>2.4489999999999998</v>
+      </c>
+      <c r="C31">
+        <f>37.7/10</f>
+        <v>3.7700000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="10">
+        <f>AVERAGE(B27,B22,B17)</f>
+        <v>75.256666666666661</v>
+      </c>
+      <c r="C32" s="7">
+        <f>AVERAGE(C27,C22,C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="7">
+        <f t="shared" ref="B33:C34" si="0">AVERAGE(B28,B23,B18)</f>
+        <v>48.73</v>
+      </c>
+      <c r="C33" s="10">
+        <f t="shared" si="0"/>
+        <v>14.227316784869977</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="7">
+        <f t="shared" si="0"/>
+        <v>58.48</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>58.48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <f>(SUM(B16:B19)*B7+SUM(C16:C19)*C7+SUM(B21:B24)*B11+SUM(C21:C24)*C11+SUM(B26:B29)*B10+SUM(C26:C29)*C10+SUM(B31:B34)*B3+SUM(C31:C34)*C3)/SUM(B3:C3,B7:C7,B10:C11)</f>
+        <v>120.76792682712498</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <f>A39*About!A27</f>
+        <v>154.34141048506572</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -690,54 +1323,56 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>154.34141048506572</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>154.34141048506572</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
land use file upload
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94B7C1-28EB-4AAB-A6C5-9A13131631C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,11 @@
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191028" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,6 +35,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,9 +51,27 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Based on consultation with the organization American Forests, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">annual ongoing for land affected by these policy levers is a </t>
+  </si>
+  <si>
+    <t>small part of lifetime costs. For this reason, we do not attempt</t>
+  </si>
+  <si>
+    <t>to track these in the US model.</t>
+  </si>
+  <si>
+    <t>annual maintenance cost ($ / acre)</t>
+  </si>
+  <si>
     <t>forest set asides</t>
   </si>
   <si>
@@ -66,31 +88,13 @@
   </si>
   <si>
     <t>forest restoration</t>
-  </si>
-  <si>
-    <t>annual maintenance cost ($ / acre)</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Based on consultation with the organization American Forests, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">annual ongoing for land affected by these policy levers is a </t>
-  </si>
-  <si>
-    <t>small part of lifetime costs. For this reason, we do not attempt</t>
-  </si>
-  <si>
-    <t>to track these in the US model.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,12 +206,10 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -232,7 +234,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -276,22 +278,16 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
-        <row r="4">
-          <cell r="A4">
-            <v>3.6666666666666665</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="19"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,9 +325,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,26 +360,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,26 +395,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -611,60 +573,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="14.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.45">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.45"/>
+    <row r="11" spans="1:2" ht="14.45"/>
+    <row r="13" spans="1:2" ht="14.45"/>
+    <row r="14" spans="1:2" ht="14.45"/>
+    <row r="15" spans="1:2" ht="14.45"/>
+    <row r="16" spans="1:2" ht="14.45"/>
+    <row r="17" spans="1:1" ht="14.45"/>
+    <row r="18" spans="1:1" ht="14.45"/>
+    <row r="19" spans="1:1" ht="14.45"/>
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
   </sheetData>
@@ -679,63 +641,63 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -744,4 +706,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EEC6ACE-C893-4C18-89E9-20287CA1E61A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE475183-E98E-4CE6-AA65-6A20911203CA}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0D0E1-FD1E-4668-93E7-815EF0DDEF4D}"/>
 </file>
</xml_diff>